<commit_message>
added data-coordinate extraction module
</commit_message>
<xml_diff>
--- a/dataprocessing/test.xlsx
+++ b/dataprocessing/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\small\Desktop\VAMAP\Team16_Development\dataprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C60B73D-400F-40D9-B479-A2B36DB70F35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F93BDA-4E25-45F8-8807-44CFDD6238AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" xr2:uid="{D02863B5-8E0E-4777-9467-E13BE1258792}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -429,7 +429,7 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -437,10 +437,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B3">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -448,10 +448,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>24</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>24</v>
@@ -481,7 +481,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>24</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>24</v>

</xml_diff>

<commit_message>
MVP of data processing. need to accelerate speed. Also need to handle exception
</commit_message>
<xml_diff>
--- a/dataprocessing/test.xlsx
+++ b/dataprocessing/test.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\small\Desktop\VAMAP\Team16_Development\dataprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F93BDA-4E25-45F8-8807-44CFDD6238AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF846A72-9518-49A3-9E37-A863E9BDADF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" xr2:uid="{D02863B5-8E0E-4777-9467-E13BE1258792}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" activeTab="2" xr2:uid="{D02863B5-8E0E-4777-9467-E13BE1258792}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -407,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9292E24D-DFD4-4470-9763-5C3B1C2D2351}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -506,4 +508,212 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C32BBA6-C3C2-4BCA-80AC-8D7B9F97B9FB}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B139A7F-4939-465F-BA18-F4FDC7E26FA4}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implement finished but need to manage strings
</commit_message>
<xml_diff>
--- a/dataprocessing/test.xlsx
+++ b/dataprocessing/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\small\Desktop\VAMAP\Team16_Development\dataprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF846A72-9518-49A3-9E37-A863E9BDADF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABB2ABF-3CC2-4BAC-9F7F-95F5AF9F09E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" activeTab="2" xr2:uid="{D02863B5-8E0E-4777-9467-E13BE1258792}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asdf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9292E24D-DFD4-4470-9763-5C3B1C2D2351}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:C8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -431,10 +443,10 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>15.1</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -445,7 +457,7 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -456,7 +468,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -464,10 +476,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -478,7 +490,7 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -489,7 +501,7 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -500,7 +512,12 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C9">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -515,7 +532,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -539,7 +556,7 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -550,7 +567,7 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -561,7 +578,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -572,7 +589,7 @@
         <v>24</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -583,7 +600,7 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -594,7 +611,7 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -605,7 +622,7 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -616,15 +633,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B139A7F-4939-465F-BA18-F4FDC7E26FA4}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,10 +649,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>23</v>
       </c>
@@ -643,10 +669,19 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>14</v>
       </c>
@@ -654,10 +689,19 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+        <v>123</v>
+      </c>
+      <c r="D3">
+        <v>123</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>24</v>
       </c>
@@ -665,21 +709,36 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>24</v>
       </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>3</v>
       </c>
@@ -687,21 +746,36 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+        <v>123412</v>
+      </c>
+      <c r="D6">
+        <v>34</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -709,11 +783,21 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished handling string, character of address. Unstable on saving data into csv. Removal of dtype occured.
</commit_message>
<xml_diff>
--- a/dataprocessing/test.xlsx
+++ b/dataprocessing/test.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\small\Desktop\VAMAP\Team16_Development\dataprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABB2ABF-3CC2-4BAC-9F7F-95F5AF9F09E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C4C987-52BF-4D05-82F6-EDD5E8EB2D4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" activeTab="2" xr2:uid="{D02863B5-8E0E-4777-9467-E13BE1258792}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" xr2:uid="{D02863B5-8E0E-4777-9467-E13BE1258792}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,15 +44,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>x2</t>
+    <t>q</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>y2</t>
+    <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>asdf</t>
+    <t>aa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -421,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9292E24D-DFD4-4470-9763-5C3B1C2D2351}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -445,8 +443,8 @@
       <c r="B2">
         <v>15.1</v>
       </c>
-      <c r="C2">
-        <v>2</v>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -456,8 +454,8 @@
       <c r="B3">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>34</v>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -467,8 +465,8 @@
       <c r="B4">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>523</v>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -478,8 +476,8 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>45</v>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -489,8 +487,8 @@
       <c r="B6">
         <v>24</v>
       </c>
-      <c r="C6">
-        <v>23</v>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -500,8 +498,8 @@
       <c r="B7">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>45</v>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -511,287 +509,12 @@
       <c r="B8">
         <v>24</v>
       </c>
-      <c r="C8">
-        <v>23</v>
+      <c r="C8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="C9">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C32BBA6-C3C2-4BCA-80AC-8D7B9F97B9FB}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>23</v>
-      </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>24</v>
-      </c>
-      <c r="C5">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>24</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>24</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>24</v>
-      </c>
-      <c r="C8">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B139A7F-4939-465F-BA18-F4FDC7E26FA4}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>23</v>
-      </c>
-      <c r="B2">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>123</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>123</v>
-      </c>
-      <c r="D3">
-        <v>123</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>23</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>24</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>24</v>
-      </c>
-      <c r="C6">
-        <v>123412</v>
-      </c>
-      <c r="D6">
-        <v>34</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>24</v>
-      </c>
-      <c r="C8">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
+      <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>